<commit_message>
Added plot_evolution_error function and visualize_functions run script
</commit_message>
<xml_diff>
--- a/tables/PSO/PSO_pop_20_w_1_c1_2_c2_2/PSO_table2_F14_dim10.xlsx
+++ b/tables/PSO/PSO_pop_20_w_1_c1_2_c2_2/PSO_table2_F14_dim10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>MaxFES</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Run 49</t>
+  </si>
+  <si>
+    <t>Run 50</t>
   </si>
   <si>
     <t>Mean</t>
@@ -523,7 +526,7 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:AZ14"/>
+  <dimension ref="A1:BA14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +534,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:52">
+    <row r="1" spans="1:53">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,8 +691,11 @@
       <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="BA1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:52">
+    <row r="2" spans="1:53">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -844,10 +850,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ2" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="3" spans="1:52">
+    <row r="3" spans="1:53">
       <c r="A3" s="1" t="n">
         <v>0.001</v>
       </c>
@@ -1002,10 +1011,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ3" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="4" spans="1:52">
+    <row r="4" spans="1:53">
       <c r="A4" s="1" t="n">
         <v>0.01</v>
       </c>
@@ -1160,10 +1172,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ4" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="5" spans="1:52">
+    <row r="5" spans="1:53">
       <c r="A5" s="1" t="n">
         <v>0.1</v>
       </c>
@@ -1318,10 +1333,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ5" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="6" spans="1:52">
+    <row r="6" spans="1:53">
       <c r="A6" s="1" t="n">
         <v>0.2</v>
       </c>
@@ -1476,10 +1494,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ6" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="7" spans="1:52">
+    <row r="7" spans="1:53">
       <c r="A7" s="1" t="n">
         <v>0.3</v>
       </c>
@@ -1634,10 +1655,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ7" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="8" spans="1:52">
+    <row r="8" spans="1:53">
       <c r="A8" s="1" t="n">
         <v>0.4</v>
       </c>
@@ -1792,10 +1816,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ8" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="9" spans="1:52">
+    <row r="9" spans="1:53">
       <c r="A9" s="1" t="n">
         <v>0.5</v>
       </c>
@@ -1950,10 +1977,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ9" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="10" spans="1:52">
+    <row r="10" spans="1:53">
       <c r="A10" s="1" t="n">
         <v>0.6</v>
       </c>
@@ -2108,10 +2138,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ10" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="11" spans="1:52">
+    <row r="11" spans="1:53">
       <c r="A11" s="1" t="n">
         <v>0.7</v>
       </c>
@@ -2266,10 +2299,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ11" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="12" spans="1:52">
+    <row r="12" spans="1:53">
       <c r="A12" s="1" t="n">
         <v>0.8</v>
       </c>
@@ -2424,10 +2460,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ12" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="13" spans="1:52">
+    <row r="13" spans="1:53">
       <c r="A13" s="1" t="n">
         <v>0.9</v>
       </c>
@@ -2582,10 +2621,13 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ13" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
-    <row r="14" spans="1:52">
+    <row r="14" spans="1:53">
       <c r="A14" s="1" t="n">
         <v>1</v>
       </c>
@@ -2740,7 +2782,10 @@
         <v>35.08640802</v>
       </c>
       <c r="AZ14" t="n">
-        <v>45.25608165</v>
+        <v>41.25852034</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>45.1776981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>